<commit_message>
adicionado arquivo banco de dados
</commit_message>
<xml_diff>
--- a/App/banco_dados.xlsx
+++ b/App/banco_dados.xlsx
@@ -250,20 +250,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -298,389 +298,389 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="19.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="18.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="9.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="n">
+      <c r="G2" s="4" t="n">
         <v>10000001</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="3" t="n">
+      <c r="G3" s="4" t="n">
         <v>10000002</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="3" t="n">
+      <c r="G4" s="4" t="n">
         <v>10000003</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="3" t="n">
+      <c r="G5" s="4" t="n">
         <v>10000004</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="3" t="n">
+      <c r="G6" s="4" t="n">
         <v>10000005</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="B7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="3" t="n">
+      <c r="G7" s="4" t="n">
         <v>10000006</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="6"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="6"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="6"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="6"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
ultimo teste realizado e tudo ok
</commit_message>
<xml_diff>
--- a/App/banco_dados.xlsx
+++ b/App/banco_dados.xlsx
@@ -619,7 +619,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
@@ -786,11 +786,15 @@
           <t>Dewaltt</t>
         </is>
       </c>
-      <c r="D3" s="26" t="n"/>
-      <c r="E3" s="28" t="n"/>
-      <c r="F3" s="29" t="n"/>
-      <c r="G3" s="29" t="n"/>
-      <c r="H3" s="27" t="n"/>
+      <c r="D3" s="26" t="inlineStr">
+        <is>
+          <t>eu</t>
+        </is>
+      </c>
+      <c r="E3" s="28" t="inlineStr"/>
+      <c r="F3" s="29" t="inlineStr"/>
+      <c r="G3" s="29" t="inlineStr"/>
+      <c r="H3" s="27" t="inlineStr"/>
       <c r="J3" s="26" t="n"/>
       <c r="K3" s="28" t="n"/>
       <c r="L3" s="28" t="n"/>
@@ -809,11 +813,15 @@
           <t>Gedore</t>
         </is>
       </c>
-      <c r="D4" s="30" t="n"/>
-      <c r="E4" s="28" t="n"/>
-      <c r="F4" s="29" t="n"/>
-      <c r="G4" s="29" t="n"/>
-      <c r="H4" s="27" t="n"/>
+      <c r="D4" s="30" t="inlineStr">
+        <is>
+          <t>Teste</t>
+        </is>
+      </c>
+      <c r="E4" s="28" t="inlineStr"/>
+      <c r="F4" s="29" t="inlineStr"/>
+      <c r="G4" s="29" t="inlineStr"/>
+      <c r="H4" s="27" t="inlineStr"/>
       <c r="J4" s="26" t="n"/>
       <c r="K4" s="28" t="n"/>
       <c r="L4" s="28" t="n"/>

</xml_diff>